<commit_message>
se agregó columna severity
</commit_message>
<xml_diff>
--- a/Ejercicio_01/Reporte_Bug_OP2.xlsx
+++ b/Ejercicio_01/Reporte_Bug_OP2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OLE HOME\CV\NTT DATA\Ejercicio_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OLE HOME\CV\NTT DATA\NTT\Ejercicio_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7793B3-10C6-4B87-A87E-EDB00B860B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA3158-2122-4F6F-89FA-D96AE91A8D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7050FA88-EB73-4950-AD7B-7C41FBEEAE54}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Issue Type</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Error de Traducción (EN) en los combobox del formulario y la descripción del Webinar.</t>
+  </si>
+  <si>
+    <t>Severidad</t>
   </si>
 </sst>
 </file>
@@ -580,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D4BC7F-6C02-47CC-85BE-6441AFD24DAD}">
-  <dimension ref="A2:P3"/>
+  <dimension ref="A2:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,12 +597,12 @@
     <col min="4" max="4" width="11.42578125" style="10"/>
     <col min="5" max="5" width="14.28515625" style="11" customWidth="1"/>
     <col min="6" max="7" width="36.140625" style="11" customWidth="1"/>
-    <col min="8" max="11" width="11.42578125" style="10"/>
-    <col min="12" max="12" width="14.42578125" style="10" customWidth="1"/>
-    <col min="13" max="16" width="11.42578125" style="10"/>
+    <col min="8" max="12" width="11.42578125" style="10"/>
+    <col min="13" max="13" width="14.42578125" style="10" customWidth="1"/>
+    <col min="14" max="17" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -628,28 +631,31 @@
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -677,25 +683,26 @@
       <c r="I3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5"/>
+      <c r="K3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="9">
+      <c r="N3" s="9">
         <v>45065</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>